<commit_message>
client info xlss updated
</commit_message>
<xml_diff>
--- a/ISSClientInfo.xlsx
+++ b/ISSClientInfo.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KG Project\ISS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A04C21D-8EE7-4B84-AC2A-1BD364B131A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52926449-C8F7-49DC-8B3F-3D7BD8A2D6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Company Name</t>
   </si>
@@ -133,6 +133,45 @@
   </si>
   <si>
     <t>17-08-2023</t>
+  </si>
+  <si>
+    <t>Mollika Updated</t>
+  </si>
+  <si>
+    <t>kg3933</t>
+  </si>
+  <si>
+    <t>MollikaDB</t>
+  </si>
+  <si>
+    <t>29-08-2023</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>ISS</t>
+  </si>
+  <si>
+    <t>Jackfruit</t>
+  </si>
+  <si>
+    <t>BondhonSeeds</t>
+  </si>
+  <si>
+    <t>BandhanSeedsDb</t>
+  </si>
+  <si>
+    <t>30-08-2023</t>
+  </si>
+  <si>
+    <t>http://103.132.94.84:125/</t>
+  </si>
+  <si>
+    <t>http://103.132.94.84:124/</t>
+  </si>
+  <si>
+    <t>31-08-2023</t>
   </si>
 </sst>
 </file>
@@ -490,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +548,7 @@
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,8 +576,11 @@
       <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -558,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>13</v>
@@ -566,8 +608,11 @@
       <c r="I2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -587,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>13</v>
@@ -595,8 +640,11 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -616,7 +664,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>13</v>
@@ -624,8 +672,11 @@
       <c r="I4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -650,11 +701,11 @@
       <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -674,40 +725,101 @@
         <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -732,13 +844,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DDA1D29B-DFC5-4C83-8788-E12B183B4AD6}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{C08430AA-07D2-4C3D-ABD1-8EF4D73E02AA}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{AC253E52-FF40-47CF-B317-588F0C6FBD38}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{578E27AF-58D1-4769-A736-F6380A9A6EC9}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{F75CA3D9-6415-4346-B337-84E4B1A4FE5A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{160C73A5-B2D1-48ED-9F14-A6F553FA260C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>